<commit_message>
Revert "Revert "create shooting""
This reverts commit 4f9752f142d26acd63bbc39775f2b08b365380f0.
</commit_message>
<xml_diff>
--- a/游戏策划.xlsx
+++ b/游戏策划.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity_Project\Sweet_Dream\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F716166A-849A-4E20-A95F-0FC794403D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00243224-FE6C-4E9F-96E4-DBA9E04E16D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="664" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="664" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="日程表" sheetId="7" r:id="rId1"/>
     <sheet name="背景策划" sheetId="1" r:id="rId2"/>
     <sheet name="遊戲機制" sheetId="9" r:id="rId3"/>
-    <sheet name="美术需求" sheetId="10" r:id="rId4"/>
-    <sheet name="系统策划" sheetId="3" r:id="rId5"/>
-    <sheet name="关卡设计" sheetId="8" r:id="rId6"/>
-    <sheet name="UI" sheetId="11" r:id="rId7"/>
-    <sheet name="时间梦境" sheetId="6" state="hidden" r:id="rId8"/>
+    <sheet name="小关卡" sheetId="12" r:id="rId4"/>
+    <sheet name="美术需求" sheetId="10" r:id="rId5"/>
+    <sheet name="系统策划" sheetId="3" r:id="rId6"/>
+    <sheet name="关卡设计" sheetId="8" r:id="rId7"/>
+    <sheet name="UI" sheetId="11" r:id="rId8"/>
+    <sheet name="时间梦境" sheetId="6" state="hidden" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="205">
   <si>
     <t>移动</t>
   </si>
@@ -265,42 +266,6 @@
     <t>劉健泓</t>
   </si>
   <si>
-    <t>遊戲目標</t>
-  </si>
-  <si>
-    <t>每個關卡都會看到白影走向某個門（提示玩家目的地）</t>
-  </si>
-  <si>
-    <t>預計遊玩時長</t>
-  </si>
-  <si>
-    <t>20-40分鐘</t>
-  </si>
-  <si>
-    <t>夢境精靈</t>
-  </si>
-  <si>
-    <t>夢境精靈會進入心靈有不安的人的夢境
-透過探索夢境
-深入到他的內心深處
-把他從不安中拯救</t>
-  </si>
-  <si>
-    <t>夢境主人</t>
-  </si>
-  <si>
-    <t>大學生，受到各種壓力壓迫</t>
-  </si>
-  <si>
-    <t>陰影</t>
-  </si>
-  <si>
-    <t>夢境的守衛，驅除外來者</t>
-  </si>
-  <si>
-    <t>關卡數</t>
-  </si>
-  <si>
     <t>THE WORLD</t>
   </si>
   <si>
@@ -496,12 +461,6 @@
     <t>镜头跟随</t>
   </si>
   <si>
-    <t>地圖</t>
-  </si>
-  <si>
-    <t>大地圖</t>
-  </si>
-  <si>
     <t>影子形態(小遊戲、解迷)</t>
   </si>
   <si>
@@ -562,20 +521,12 @@
     <t>綿羊</t>
   </si>
   <si>
-    <t>梦境</t>
-  </si>
-  <si>
     <t>散架平台</t>
   </si>
   <si>
     <t>向上泡泡</t>
   </si>
   <si>
-    <t xml:space="preserve">表層夢境
-深層夢境
-</t>
-  </si>
-  <si>
     <t>電梯</t>
   </si>
   <si>
@@ -606,9 +557,6 @@
     <t>Resume</t>
   </si>
   <si>
-    <t>以夢境的各種機關來解迷和戰鬥2d橫版遊戲</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
@@ -618,9 +566,6 @@
     <t>完成</t>
   </si>
   <si>
-    <t>追上一個白影（夢境主人）\ 收集蝴蝶</t>
-  </si>
-  <si>
     <t>接近縮放</t>
   </si>
   <si>
@@ -634,6 +579,84 @@
   </si>
   <si>
     <t>尖刺荊棘</t>
+  </si>
+  <si>
+    <t>透过跑酷和解谜深入主人的梦境，打败其梦境的阴影</t>
+  </si>
+  <si>
+    <t>游戏目标</t>
+  </si>
+  <si>
+    <t>游戏简介</t>
+  </si>
+  <si>
+    <t>本作是一款2d平台跳跃游戏，玩家会扮演梦境精灵，在大地图中跑酷进入5个小房间，在五个房间中，玩家将会看到梦境主人的经历、内心渴望等。随着探索的深入，玩家会逐渐进入梦境主人的深层梦境，玩家将会遇见更强大的敌人和怪物，最终进入主人梦境的最深处，打败他内心的阴影，拯救陷入焦虑不安中的主人</t>
+  </si>
+  <si>
+    <t>梦境精灵</t>
+  </si>
+  <si>
+    <t>梦境精灵会进入心灵有不安的人的梦境
+透过探索梦境
+深入到他的内心深处
+把他从不安中拯救</t>
+  </si>
+  <si>
+    <t>梦境主人</t>
+  </si>
+  <si>
+    <t>大学生，受到各种压力压迫</t>
+  </si>
+  <si>
+    <t>阴影</t>
+  </si>
+  <si>
+    <t>梦境的守卫，驱除外来者</t>
+  </si>
+  <si>
+    <t>预计游玩时长</t>
+  </si>
+  <si>
+    <t>20-40分钟</t>
+  </si>
+  <si>
+    <t>关卡数</t>
+  </si>
+  <si>
+    <t>地图</t>
+  </si>
+  <si>
+    <t>大地图</t>
+  </si>
+  <si>
+    <t>微信</t>
+  </si>
+  <si>
+    <t>监狱</t>
+  </si>
+  <si>
+    <t>夹子</t>
+  </si>
+  <si>
+    <t>灯光杀</t>
+  </si>
+  <si>
+    <t>左右移动平台</t>
+  </si>
+  <si>
+    <t>推箱子</t>
+  </si>
+  <si>
+    <t>踩到指定平台</t>
+  </si>
+  <si>
+    <t>钥匙/门</t>
+  </si>
+  <si>
+    <t>以夢境的各種機關來解迷和戰鬥2d橫版跑酷遊戲</t>
+  </si>
+  <si>
+    <t>SavePoint</t>
   </si>
 </sst>
 </file>
@@ -704,7 +727,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -735,6 +758,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1014,7 +1040,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.2"/>
@@ -1133,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="19.8"/>
@@ -1147,94 +1173,85 @@
     <col min="4" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="78" customHeight="1">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="103.8" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" ht="79.2">
       <c r="A2" s="3" t="s">
-        <v>79</v>
+        <v>184</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>80</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="33.6" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>81</v>
+        <v>186</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>82</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="27" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>188</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>84</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.2" customHeight="1">
       <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="10" t="s">
-        <v>75</v>
+      <c r="A6" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>78</v>
+        <v>192</v>
+      </c>
+      <c r="B8" s="5">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>152</v>
+        <v>193</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A6:A7"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F4EBE1-4F98-49D0-957C-BCBA222D8DD6}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.375" defaultRowHeight="19.8"/>
@@ -1246,207 +1263,252 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="39.6">
       <c r="A2" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>157</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="7"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="5" t="s">
-        <v>101</v>
+      <c r="A4" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="10"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="5" t="s">
-        <v>158</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="10"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="13"/>
+      <c r="B7" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="5" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="13"/>
+      <c r="B8" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="13"/>
+      <c r="B9" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="13"/>
+      <c r="B10" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="13"/>
+      <c r="B11" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="13"/>
+      <c r="B12" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="13"/>
+      <c r="B13" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="13"/>
+      <c r="B14" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="13"/>
+      <c r="B15" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="13"/>
+      <c r="B16" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="10" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="10"/>
-      <c r="B16" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="10"/>
       <c r="B25" s="1" t="s">
-        <v>109</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="10"/>
       <c r="B26" s="1" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="10" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>154</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="10"/>
       <c r="B28" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="10"/>
+      <c r="B30" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="10"/>
+      <c r="B31" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="10"/>
+      <c r="B32" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="10"/>
+      <c r="B33" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="10"/>
+      <c r="B34" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="10"/>
+      <c r="B36" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="10"/>
+      <c r="B37" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="10"/>
-      <c r="B29" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>179</v>
+      <c r="B40" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A3:A16"/>
+  <mergeCells count="4">
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1454,11 +1516,39 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351EE840-3FF0-4F96-940A-6A3B5E94EA7E}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="56.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D59B53-E025-472E-AA4F-CA221093659D}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.6"/>
@@ -1471,13 +1561,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="11" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1486,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1495,7 +1585,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1507,55 +1597,55 @@
     <row r="5" spans="1:3">
       <c r="A5" s="11"/>
       <c r="B5" s="8" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="11"/>
       <c r="B6" s="8" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="11"/>
       <c r="B7" s="8" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="11" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="11"/>
       <c r="B9" s="8" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="25.2" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="27.6" customHeight="1">
       <c r="A11" s="11"/>
       <c r="B11" s="8" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="11" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>29</v>
@@ -1570,60 +1660,60 @@
     <row r="14" spans="1:3">
       <c r="A14" s="11"/>
       <c r="B14" s="8" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="11"/>
       <c r="B15" s="8" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="11"/>
       <c r="B16" s="8" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="11"/>
       <c r="B17" s="8" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="11"/>
       <c r="B18" s="8" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="11"/>
       <c r="B19" s="8" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="11"/>
       <c r="B20" s="8" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="11"/>
       <c r="B21" s="8" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="11"/>
       <c r="B22" s="8" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="11" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>38</v>
@@ -1638,7 +1728,7 @@
     <row r="25" spans="1:2">
       <c r="A25" s="11"/>
       <c r="B25" s="8" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1654,11 +1744,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1673,13 +1763,13 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="10" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1694,7 +1784,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -1709,7 +1799,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -1736,24 +1826,24 @@
     <row r="5" spans="1:6">
       <c r="A5" s="10"/>
       <c r="B5" s="1" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="10" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
@@ -1762,10 +1852,10 @@
     <row r="7" spans="1:6">
       <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -1780,7 +1870,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>51</v>
@@ -1792,57 +1882,57 @@
     <row r="9" spans="1:6" ht="22.2" customHeight="1">
       <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="22.2" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="1" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="22.2" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="22.2" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="1" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="22.2" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="1" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="22.2" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="1" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="22.2" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
@@ -1860,7 +1950,7 @@
         <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1869,18 +1959,18 @@
         <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="10"/>
       <c r="B19" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="22.2" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>21</v>
@@ -1892,30 +1982,30 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="22.2" customHeight="1">
       <c r="A22" s="10"/>
       <c r="B22" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="22.2" customHeight="1">
       <c r="A23" s="10"/>
       <c r="B23" s="1" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="22.2" customHeight="1">
       <c r="B24" s="1" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1929,7 +2019,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3997C269-5D82-4F85-AB85-A817CF582DB6}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1947,65 +2037,65 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2014,11 +2104,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B0EF9D-A917-4976-A985-BA52013DC77B}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2031,48 +2121,48 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="10" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="10"/>
       <c r="B2" s="1" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="10"/>
       <c r="B3" s="1" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="10"/>
       <c r="B4" s="1" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="10" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="10"/>
       <c r="B6" s="1" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2084,7 +2174,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -2102,7 +2192,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="100.2" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>24</v>
@@ -2184,17 +2274,17 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2204,7 +2294,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="4" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2239,33 +2329,33 @@
         <v>53</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="4" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="4" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="C22" s="4" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="B23" s="4" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hit effect and time stop
</commit_message>
<xml_diff>
--- a/游戏策划.xlsx
+++ b/游戏策划.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity_Project\Sweet_Dream\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE9F483-309D-4614-BCCC-21857E701F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B3A9F2-412B-41CF-9CC9-0F335FC4B930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="664" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="664" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="日程表" sheetId="7" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="小关卡" sheetId="12" r:id="rId5"/>
     <sheet name="美术需求" sheetId="10" r:id="rId6"/>
     <sheet name="系统策划" sheetId="3" r:id="rId7"/>
-    <sheet name="关卡设计" sheetId="8" r:id="rId8"/>
-    <sheet name="UI" sheetId="11" r:id="rId9"/>
-    <sheet name="时间梦境" sheetId="6" state="hidden" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="14" r:id="rId8"/>
+    <sheet name="关卡设计" sheetId="8" r:id="rId9"/>
+    <sheet name="UI" sheetId="11" r:id="rId10"/>
+    <sheet name="时间梦境" sheetId="6" state="hidden" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="249">
   <si>
     <t>移动</t>
   </si>
@@ -772,6 +773,24 @@
   </si>
   <si>
     <t xml:space="preserve"> 加速/时间停止/追逐</t>
+  </si>
+  <si>
+    <t>旋轉</t>
+  </si>
+  <si>
+    <t>冰(温度)</t>
+  </si>
+  <si>
+    <t>聊天記錄</t>
+  </si>
+  <si>
+    <t>分數GPA</t>
+  </si>
+  <si>
+    <t>移動(單個/多個)</t>
+  </si>
+  <si>
+    <t>日月改變(温度)(明暗障礙物)</t>
   </si>
 </sst>
 </file>
@@ -1281,6 +1300,104 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B0EF9D-A917-4976-A985-BA52013DC77B}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="19.8"/>
+  <cols>
+    <col min="1" max="1" width="31.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.25" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12"/>
+      <c r="B4" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12"/>
+      <c r="B6" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="12"/>
+      <c r="B7" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="12"/>
+      <c r="B10" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -1479,7 +1596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D914EB04-9B35-404C-B40B-50CA7A01795A}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -1726,8 +1843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F4EBE1-4F98-49D0-957C-BCBA222D8DD6}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.375" defaultRowHeight="19.8"/>
@@ -2023,7 +2140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D59B53-E025-472E-AA4F-CA221093659D}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -2225,7 +2342,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView zoomScale="86" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="19.8"/>
@@ -2496,11 +2613,70 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C90C87E-AFF8-4BE9-A25B-802E8A5FF7BE}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="22.2"/>
+  <cols>
+    <col min="1" max="1" width="71.125" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3997C269-5D82-4F85-AB85-A817CF582DB6}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.8"/>
@@ -2578,102 +2754,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B0EF9D-A917-4976-A985-BA52013DC77B}">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.8"/>
-  <cols>
-    <col min="1" max="1" width="31.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.25" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>